<commit_message>
Results from July 19, 2020 09:35:30 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-19.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-19.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O47"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -572,13 +572,13 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44030</v>
+        <v>44031</v>
       </c>
       <c r="C3" t="n">
-        <v>28633</v>
+        <v>30835</v>
       </c>
       <c r="D3" t="n">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="E3" t="n">
         <v>464</v>
@@ -728,26 +728,44 @@
           <t>California - San Francisco</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+      <c r="B6" s="2" t="n">
+        <v>44030</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5202</v>
+      </c>
+      <c r="D6" t="n">
+        <v>43</v>
+      </c>
+      <c r="E6" t="n">
+        <v>283</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>6.32</v>
+      </c>
+      <c r="H6" t="n">
+        <v>12.2</v>
+      </c>
       <c r="I6" t="b">
         <v>0</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
       </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
+      <c r="K6" t="n">
+        <v>4481</v>
+      </c>
+      <c r="L6" t="n">
+        <v>41</v>
+      </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr">
         <is>
-          <t>An error occurred. ... AttributeError("'NoneType' object has no attribute 'body'")</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -912,19 +930,19 @@
         <v>44031</v>
       </c>
       <c r="C10" t="n">
-        <v>32533</v>
+        <v>33228</v>
       </c>
       <c r="D10" t="n">
         <v>357</v>
       </c>
       <c r="E10" t="n">
-        <v>6918</v>
+        <v>7041</v>
       </c>
       <c r="F10" t="n">
         <v>93</v>
       </c>
       <c r="G10" t="n">
-        <v>24.53</v>
+        <v>24.59</v>
       </c>
       <c r="H10" t="n">
         <v>26.2</v>
@@ -936,7 +954,7 @@
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>28197</v>
+        <v>28631</v>
       </c>
       <c r="L10" t="n">
         <v>355</v>
@@ -960,16 +978,16 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44030</v>
+        <v>44031</v>
       </c>
       <c r="C11" t="n">
-        <v>23114</v>
+        <v>23682</v>
       </c>
       <c r="D11" t="n">
         <v>478</v>
       </c>
       <c r="E11" t="n">
-        <v>847</v>
+        <v>864</v>
       </c>
       <c r="F11" t="n">
         <v>18</v>
@@ -987,7 +1005,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>18089</v>
+        <v>18459</v>
       </c>
       <c r="L11" t="n">
         <v>462</v>
@@ -1242,22 +1260,22 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44029</v>
+        <v>44030</v>
       </c>
       <c r="C17" t="n">
-        <v>153041</v>
+        <v>155887</v>
       </c>
       <c r="D17" t="n">
-        <v>4084</v>
+        <v>4095</v>
       </c>
       <c r="E17" t="n">
-        <v>4094</v>
+        <v>4162</v>
       </c>
       <c r="F17" t="n">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="G17" t="n">
-        <v>4.69</v>
+        <v>4.67</v>
       </c>
       <c r="H17" t="n">
         <v>10.76</v>
@@ -1269,10 +1287,10 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>87304</v>
+        <v>89087</v>
       </c>
       <c r="L17" t="n">
-        <v>3801</v>
+        <v>3812</v>
       </c>
       <c r="M17" t="n">
         <v>823987</v>
@@ -1343,18 +1361,32 @@
           <t>Mississippi</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+      <c r="B19" s="2" t="n">
+        <v>44030</v>
+      </c>
+      <c r="C19" t="n">
+        <v>42638</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1355</v>
+      </c>
+      <c r="E19" t="n">
+        <v>19470</v>
+      </c>
+      <c r="F19" t="n">
+        <v>678</v>
+      </c>
+      <c r="G19" t="n">
+        <v>45.66</v>
+      </c>
+      <c r="H19" t="n">
+        <v>50.04</v>
+      </c>
       <c r="I19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
@@ -1366,54 +1398,54 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>An error occurred. ... AttributeError("'NoneType' object has no attribute 'groups'")</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Pennsylvania</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C20" t="n">
-        <v>98164</v>
+        <v>143624</v>
       </c>
       <c r="D20" t="n">
-        <v>7015</v>
+        <v>2761</v>
       </c>
       <c r="E20" t="n">
-        <v>13749</v>
+        <v>3102</v>
       </c>
       <c r="F20" t="n">
-        <v>1484</v>
+        <v>81</v>
       </c>
       <c r="G20" t="n">
-        <v>30.22</v>
+        <v>4.32</v>
       </c>
       <c r="H20" t="n">
-        <v>21.22</v>
+        <v>3.48</v>
       </c>
       <c r="I20" t="b">
         <v>0</v>
       </c>
       <c r="J20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>45500</v>
+        <v>71888</v>
       </c>
       <c r="L20" t="n">
-        <v>6992</v>
+        <v>2325</v>
       </c>
       <c r="M20" t="n">
-        <v>1423319</v>
+        <v>305259</v>
       </c>
       <c r="N20" t="n">
-        <v>11.13</v>
+        <v>4.39</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1424,43 +1456,47 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Pennsylvania</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C21" t="n">
-        <v>345612</v>
+        <v>98164</v>
       </c>
       <c r="D21" t="n">
-        <v>4982</v>
+        <v>7015</v>
       </c>
       <c r="E21" t="n">
-        <v>41950</v>
+        <v>13749</v>
       </c>
       <c r="F21" t="n">
-        <v>945</v>
+        <v>1484</v>
       </c>
       <c r="G21" t="n">
-        <v>12.14</v>
+        <v>30.22</v>
       </c>
       <c r="H21" t="n">
-        <v>18.97</v>
+        <v>21.22</v>
       </c>
       <c r="I21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K21" t="n">
+        <v>45500</v>
+      </c>
+      <c r="L21" t="n">
+        <v>6992</v>
+      </c>
       <c r="M21" t="n">
-        <v>3316376</v>
+        <v>1423319</v>
       </c>
       <c r="N21" t="n">
-        <v>16.1</v>
+        <v>11.13</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -1471,39 +1507,43 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Montana</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C22" t="n">
-        <v>2533</v>
+        <v>345612</v>
       </c>
       <c r="D22" t="n">
-        <v>37</v>
+        <v>4982</v>
       </c>
       <c r="E22" t="n">
-        <v>13</v>
-      </c>
-      <c r="F22" t="inlineStr"/>
+        <v>41950</v>
+      </c>
+      <c r="F22" t="n">
+        <v>945</v>
+      </c>
       <c r="G22" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="H22" t="inlineStr"/>
+        <v>12.14</v>
+      </c>
+      <c r="H22" t="n">
+        <v>18.97</v>
+      </c>
       <c r="I22" t="b">
         <v>1</v>
       </c>
       <c r="J22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="n">
-        <v>4630</v>
+        <v>3316376</v>
       </c>
       <c r="N22" t="n">
-        <v>0.44</v>
+        <v>16.1</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -1514,47 +1554,39 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Vermont</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C23" t="n">
-        <v>1350</v>
+        <v>2533</v>
       </c>
       <c r="D23" t="n">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E23" t="n">
-        <v>150</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
-        <v>11.44</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0</v>
-      </c>
+        <v>0.51</v>
+      </c>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="b">
         <v>1</v>
       </c>
-      <c r="K23" t="n">
-        <v>1311</v>
-      </c>
-      <c r="L23" t="n">
-        <v>56</v>
-      </c>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
       <c r="M23" t="n">
-        <v>8058</v>
+        <v>4630</v>
       </c>
       <c r="N23" t="n">
-        <v>1.29</v>
+        <v>0.44</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -1565,43 +1597,47 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Connecticut</t>
+          <t>Vermont</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>44028</v>
+        <v>44031</v>
       </c>
       <c r="C24" t="n">
-        <v>45910</v>
+        <v>1350</v>
       </c>
       <c r="D24" t="n">
-        <v>3519</v>
+        <v>56</v>
       </c>
       <c r="E24" t="n">
-        <v>6278</v>
+        <v>150</v>
       </c>
       <c r="F24" t="n">
-        <v>651</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>13.67</v>
+        <v>11.44</v>
       </c>
       <c r="H24" t="n">
-        <v>18.5</v>
+        <v>0</v>
       </c>
       <c r="I24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="b">
-        <v>0</v>
-      </c>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K24" t="n">
+        <v>1311</v>
+      </c>
+      <c r="L24" t="n">
+        <v>56</v>
+      </c>
       <c r="M24" t="n">
-        <v>378262</v>
+        <v>8058</v>
       </c>
       <c r="N24" t="n">
-        <v>10.56</v>
+        <v>1.29</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -1612,47 +1648,43 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>Connecticut</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>44029</v>
+        <v>44028</v>
       </c>
       <c r="C25" t="n">
-        <v>21965</v>
+        <v>45910</v>
       </c>
       <c r="D25" t="n">
-        <v>299</v>
+        <v>3519</v>
       </c>
       <c r="E25" t="n">
-        <v>1644</v>
+        <v>6278</v>
       </c>
       <c r="F25" t="n">
-        <v>64</v>
+        <v>651</v>
       </c>
       <c r="G25" t="n">
-        <v>9.18</v>
+        <v>13.67</v>
       </c>
       <c r="H25" t="n">
-        <v>21.99</v>
+        <v>18.5</v>
       </c>
       <c r="I25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="b">
-        <v>1</v>
-      </c>
-      <c r="K25" t="n">
-        <v>17913</v>
-      </c>
-      <c r="L25" t="n">
-        <v>291</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
       <c r="M25" t="n">
-        <v>169801</v>
+        <v>378262</v>
       </c>
       <c r="N25" t="n">
-        <v>5.84</v>
+        <v>10.56</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -1663,47 +1695,47 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>44031</v>
+        <v>44029</v>
       </c>
       <c r="C26" t="n">
-        <v>40142</v>
+        <v>21965</v>
       </c>
       <c r="D26" t="n">
-        <v>1752</v>
+        <v>299</v>
       </c>
       <c r="E26" t="n">
-        <v>1995</v>
+        <v>1644</v>
       </c>
       <c r="F26" t="n">
-        <v>118</v>
+        <v>64</v>
       </c>
       <c r="G26" t="n">
-        <v>6.25</v>
+        <v>9.18</v>
       </c>
       <c r="H26" t="n">
-        <v>6.96</v>
+        <v>21.99</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
       </c>
       <c r="J26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>31937</v>
+        <v>17913</v>
       </c>
       <c r="L26" t="n">
-        <v>1695</v>
+        <v>291</v>
       </c>
       <c r="M26" t="n">
-        <v>227938</v>
+        <v>169801</v>
       </c>
       <c r="N26" t="n">
-        <v>4.12</v>
+        <v>5.84</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -1714,47 +1746,47 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>44030</v>
+        <v>44031</v>
       </c>
       <c r="C27" t="n">
-        <v>22481</v>
+        <v>40142</v>
       </c>
       <c r="D27" t="n">
-        <v>301</v>
+        <v>1752</v>
       </c>
       <c r="E27" t="n">
-        <v>1297</v>
+        <v>1995</v>
       </c>
       <c r="F27" t="n">
-        <v>22</v>
+        <v>118</v>
       </c>
       <c r="G27" t="n">
-        <v>7.55</v>
+        <v>6.25</v>
       </c>
       <c r="H27" t="n">
-        <v>7.69</v>
+        <v>6.96</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
       </c>
       <c r="J27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>17187</v>
+        <v>31937</v>
       </c>
       <c r="L27" t="n">
-        <v>286</v>
+        <v>1695</v>
       </c>
       <c r="M27" t="n">
-        <v>90860</v>
+        <v>227938</v>
       </c>
       <c r="N27" t="n">
-        <v>4.77</v>
+        <v>4.12</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -1765,43 +1797,47 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C28" t="n">
-        <v>73575</v>
+        <v>22583</v>
       </c>
       <c r="D28" t="n">
-        <v>6041</v>
+        <v>301</v>
       </c>
       <c r="E28" t="n">
-        <v>21288</v>
+        <v>1350</v>
       </c>
       <c r="F28" t="n">
-        <v>2406</v>
+        <v>22</v>
       </c>
       <c r="G28" t="n">
-        <v>28.93</v>
+        <v>7.64</v>
       </c>
       <c r="H28" t="n">
-        <v>39.83</v>
+        <v>7.64</v>
       </c>
       <c r="I28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K28" t="n">
+        <v>17675</v>
+      </c>
+      <c r="L28" t="n">
+        <v>288</v>
+      </c>
       <c r="M28" t="n">
-        <v>1375424</v>
+        <v>90860</v>
       </c>
       <c r="N28" t="n">
-        <v>13.81</v>
+        <v>4.77</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -1812,47 +1848,43 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>44027</v>
+        <v>44031</v>
       </c>
       <c r="C29" t="n">
-        <v>91706</v>
+        <v>73575</v>
       </c>
       <c r="D29" t="n">
-        <v>3433</v>
+        <v>6041</v>
       </c>
       <c r="E29" t="n">
-        <v>32137</v>
+        <v>21288</v>
       </c>
       <c r="F29" t="n">
-        <v>1724</v>
+        <v>2406</v>
       </c>
       <c r="G29" t="n">
-        <v>48.31</v>
+        <v>28.93</v>
       </c>
       <c r="H29" t="n">
-        <v>51.56</v>
+        <v>39.83</v>
       </c>
       <c r="I29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="b">
-        <v>1</v>
-      </c>
-      <c r="K29" t="n">
-        <v>66518</v>
-      </c>
-      <c r="L29" t="n">
-        <v>3344</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
       <c r="M29" t="n">
-        <v>1502916</v>
+        <v>1375424</v>
       </c>
       <c r="N29" t="n">
-        <v>32.23</v>
+        <v>13.81</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -1863,47 +1895,47 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>California</t>
-        </is>
-      </c>
-      <c r="B30" s="3" t="n">
-        <v>44030</v>
+          <t>Louisiana</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>44027</v>
       </c>
       <c r="C30" t="n">
-        <v>384692</v>
+        <v>91706</v>
       </c>
       <c r="D30" t="n">
-        <v>7685</v>
+        <v>3433</v>
       </c>
       <c r="E30" t="n">
-        <v>10678</v>
+        <v>32137</v>
       </c>
       <c r="F30" t="n">
-        <v>654</v>
+        <v>1724</v>
       </c>
       <c r="G30" t="n">
-        <v>4.32</v>
+        <v>48.31</v>
       </c>
       <c r="H30" t="n">
-        <v>8.720000000000001</v>
+        <v>51.56</v>
       </c>
       <c r="I30" t="b">
         <v>0</v>
       </c>
       <c r="J30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" t="n">
-        <v>247369</v>
+        <v>66518</v>
       </c>
       <c r="L30" t="n">
-        <v>7501</v>
+        <v>3344</v>
       </c>
       <c r="M30" t="n">
-        <v>2267875</v>
+        <v>1502916</v>
       </c>
       <c r="N30" t="n">
-        <v>5.79</v>
+        <v>32.23</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -1914,43 +1946,47 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Indiana</t>
-        </is>
-      </c>
-      <c r="B31" s="2" t="n">
-        <v>44031</v>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>44030</v>
       </c>
       <c r="C31" t="n">
-        <v>56571</v>
+        <v>384692</v>
       </c>
       <c r="D31" t="n">
-        <v>2629</v>
+        <v>7685</v>
       </c>
       <c r="E31" t="n">
-        <v>6564</v>
+        <v>10678</v>
       </c>
       <c r="F31" t="n">
-        <v>373</v>
+        <v>654</v>
       </c>
       <c r="G31" t="n">
-        <v>11.6</v>
+        <v>4.32</v>
       </c>
       <c r="H31" t="n">
-        <v>14.19</v>
+        <v>8.720000000000001</v>
       </c>
       <c r="I31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="b">
-        <v>1</v>
-      </c>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>247369</v>
+      </c>
+      <c r="L31" t="n">
+        <v>7501</v>
+      </c>
       <c r="M31" t="n">
-        <v>619472</v>
+        <v>2267875</v>
       </c>
       <c r="N31" t="n">
-        <v>9.33</v>
+        <v>5.79</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -1961,47 +1997,43 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Alaska</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C32" t="n">
-        <v>1874</v>
+        <v>56571</v>
       </c>
       <c r="D32" t="n">
-        <v>18</v>
+        <v>2629</v>
       </c>
       <c r="E32" t="n">
-        <v>45</v>
+        <v>6564</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>373</v>
       </c>
       <c r="G32" t="n">
-        <v>1.44</v>
+        <v>11.6</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>14.19</v>
       </c>
       <c r="I32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" t="b">
         <v>1</v>
       </c>
-      <c r="K32" t="n">
-        <v>3116</v>
-      </c>
-      <c r="L32" t="n">
-        <v>36</v>
-      </c>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
       <c r="M32" t="n">
-        <v>24129</v>
+        <v>619472</v>
       </c>
       <c r="N32" t="n">
-        <v>3.27</v>
+        <v>9.33</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2012,29 +2044,29 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Alaska</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C33" t="n">
-        <v>42315</v>
+        <v>1874</v>
       </c>
       <c r="D33" t="n">
-        <v>844</v>
+        <v>18</v>
       </c>
       <c r="E33" t="n">
-        <v>6824</v>
+        <v>45</v>
       </c>
       <c r="F33" t="n">
-        <v>196</v>
+        <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>17.86</v>
+        <v>3.62</v>
       </c>
       <c r="H33" t="n">
-        <v>23.61</v>
+        <v>0</v>
       </c>
       <c r="I33" t="b">
         <v>0</v>
@@ -2043,16 +2075,16 @@
         <v>1</v>
       </c>
       <c r="K33" t="n">
-        <v>38198</v>
+        <v>1242</v>
       </c>
       <c r="L33" t="n">
-        <v>830</v>
+        <v>18</v>
       </c>
       <c r="M33" t="n">
-        <v>368744</v>
+        <v>24129</v>
       </c>
       <c r="N33" t="n">
-        <v>6.38</v>
+        <v>3.27</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2063,43 +2095,47 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C34" t="n">
-        <v>143123</v>
+        <v>42315</v>
       </c>
       <c r="D34" t="n">
-        <v>3173</v>
+        <v>844</v>
       </c>
       <c r="E34" t="n">
-        <v>36959</v>
+        <v>6824</v>
       </c>
       <c r="F34" t="n">
-        <v>1472</v>
+        <v>196</v>
       </c>
       <c r="G34" t="n">
-        <v>25.82</v>
+        <v>17.86</v>
       </c>
       <c r="H34" t="n">
-        <v>46.39</v>
+        <v>23.61</v>
       </c>
       <c r="I34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="b">
         <v>1</v>
       </c>
-      <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr"/>
+      <c r="K34" t="n">
+        <v>38198</v>
+      </c>
+      <c r="L34" t="n">
+        <v>830</v>
+      </c>
       <c r="M34" t="n">
-        <v>3239300</v>
+        <v>368744</v>
       </c>
       <c r="N34" t="n">
-        <v>31.46</v>
+        <v>6.38</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -2110,47 +2146,43 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>44030</v>
+        <v>44031</v>
       </c>
       <c r="C35" t="n">
-        <v>46026</v>
+        <v>143123</v>
       </c>
       <c r="D35" t="n">
-        <v>1444</v>
+        <v>3173</v>
       </c>
       <c r="E35" t="n">
-        <v>1690</v>
+        <v>36959</v>
       </c>
       <c r="F35" t="n">
-        <v>48</v>
+        <v>1472</v>
       </c>
       <c r="G35" t="n">
-        <v>5.42</v>
+        <v>25.82</v>
       </c>
       <c r="H35" t="n">
-        <v>3.46</v>
+        <v>46.39</v>
       </c>
       <c r="I35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" t="b">
-        <v>0</v>
-      </c>
-      <c r="K35" t="n">
-        <v>31176</v>
-      </c>
-      <c r="L35" t="n">
-        <v>1386</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
       <c r="M35" t="n">
-        <v>269854</v>
+        <v>3239300</v>
       </c>
       <c r="N35" t="n">
-        <v>3.7</v>
+        <v>31.46</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -2161,29 +2193,29 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>New Hampshire</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C36" t="n">
-        <v>6203</v>
+        <v>46946</v>
       </c>
       <c r="D36" t="n">
-        <v>398</v>
+        <v>1447</v>
       </c>
       <c r="E36" t="n">
-        <v>320</v>
+        <v>1696</v>
       </c>
       <c r="F36" t="n">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="G36" t="n">
-        <v>6.03</v>
+        <v>5.42</v>
       </c>
       <c r="H36" t="n">
-        <v>2.27</v>
+        <v>3.46</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
@@ -2192,16 +2224,16 @@
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>5308</v>
+        <v>31275</v>
       </c>
       <c r="L36" t="n">
-        <v>397</v>
+        <v>1387</v>
       </c>
       <c r="M36" t="n">
-        <v>20516</v>
+        <v>269854</v>
       </c>
       <c r="N36" t="n">
-        <v>1.53</v>
+        <v>3.7</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -2212,43 +2244,47 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Washington, DC</t>
+          <t>New Hampshire</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C37" t="n">
-        <v>11261</v>
+        <v>6203</v>
       </c>
       <c r="D37" t="n">
-        <v>578</v>
+        <v>398</v>
       </c>
       <c r="E37" t="n">
-        <v>5550</v>
+        <v>320</v>
       </c>
       <c r="F37" t="n">
-        <v>426</v>
+        <v>9</v>
       </c>
       <c r="G37" t="n">
-        <v>49.29</v>
+        <v>6.03</v>
       </c>
       <c r="H37" t="n">
-        <v>73.7</v>
+        <v>2.27</v>
       </c>
       <c r="I37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="b">
-        <v>1</v>
-      </c>
-      <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>5308</v>
+      </c>
+      <c r="L37" t="n">
+        <v>397</v>
+      </c>
       <c r="M37" t="n">
-        <v>321317</v>
+        <v>20516</v>
       </c>
       <c r="N37" t="n">
-        <v>46.94</v>
+        <v>1.53</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -2259,43 +2295,43 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>Washington, DC</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C38" t="n">
-        <v>13519</v>
+        <v>11261</v>
       </c>
       <c r="D38" t="n">
-        <v>523</v>
+        <v>578</v>
       </c>
       <c r="E38" t="n">
-        <v>3443</v>
+        <v>5550</v>
       </c>
       <c r="F38" t="n">
-        <v>134</v>
+        <v>426</v>
       </c>
       <c r="G38" t="n">
-        <v>25.47</v>
+        <v>49.29</v>
       </c>
       <c r="H38" t="n">
-        <v>25.62</v>
+        <v>73.7</v>
       </c>
       <c r="I38" t="b">
         <v>1</v>
       </c>
       <c r="J38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="n">
-        <v>209892</v>
+        <v>321317</v>
       </c>
       <c r="N38" t="n">
-        <v>22.11</v>
+        <v>46.94</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -2306,41 +2342,43 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Maine</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C39" t="n">
-        <v>3687</v>
+        <v>13519</v>
       </c>
       <c r="D39" t="n">
-        <v>117</v>
+        <v>523</v>
       </c>
       <c r="E39" t="n">
-        <v>839</v>
-      </c>
-      <c r="F39" t="inlineStr"/>
+        <v>3443</v>
+      </c>
+      <c r="F39" t="n">
+        <v>134</v>
+      </c>
       <c r="G39" t="n">
         <v>25.47</v>
       </c>
-      <c r="H39" t="inlineStr"/>
+      <c r="H39" t="n">
+        <v>25.62</v>
+      </c>
       <c r="I39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" t="b">
-        <v>1</v>
-      </c>
-      <c r="K39" t="n">
-        <v>3294</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="n">
-        <v>17881</v>
+        <v>209892</v>
       </c>
       <c r="N39" t="n">
-        <v>1.34</v>
+        <v>22.11</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -2351,43 +2389,41 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>Maine</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C40" t="n">
-        <v>38723</v>
+        <v>3687</v>
       </c>
       <c r="D40" t="n">
-        <v>793</v>
+        <v>117</v>
       </c>
       <c r="E40" t="n">
-        <v>3209</v>
-      </c>
-      <c r="F40" t="n">
-        <v>38</v>
-      </c>
+        <v>839</v>
+      </c>
+      <c r="F40" t="inlineStr"/>
       <c r="G40" t="n">
-        <v>8.289999999999999</v>
-      </c>
-      <c r="H40" t="n">
-        <v>4.79</v>
-      </c>
+        <v>25.47</v>
+      </c>
+      <c r="H40" t="inlineStr"/>
       <c r="I40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="b">
         <v>1</v>
       </c>
-      <c r="K40" t="inlineStr"/>
+      <c r="K40" t="n">
+        <v>3294</v>
+      </c>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="n">
-        <v>109911</v>
+        <v>17881</v>
       </c>
       <c r="N40" t="n">
-        <v>3.51</v>
+        <v>1.34</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -2398,47 +2434,43 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="B41" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C41" t="n">
-        <v>99778</v>
+        <v>38813</v>
       </c>
       <c r="D41" t="n">
-        <v>1634</v>
+        <v>793</v>
       </c>
       <c r="E41" t="n">
-        <v>16174</v>
+        <v>3210</v>
       </c>
       <c r="F41" t="n">
-        <v>517</v>
+        <v>38</v>
       </c>
       <c r="G41" t="n">
-        <v>23.92</v>
+        <v>8.27</v>
       </c>
       <c r="H41" t="n">
-        <v>32.76</v>
+        <v>4.79</v>
       </c>
       <c r="I41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="b">
         <v>1</v>
       </c>
-      <c r="K41" t="n">
-        <v>67629</v>
-      </c>
-      <c r="L41" t="n">
-        <v>1578</v>
-      </c>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
       <c r="M41" t="n">
-        <v>2179622</v>
+        <v>109911</v>
       </c>
       <c r="N41" t="n">
-        <v>21.46</v>
+        <v>3.51</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -2449,43 +2481,47 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C42" t="n">
-        <v>161575</v>
+        <v>99778</v>
       </c>
       <c r="D42" t="n">
-        <v>7295</v>
+        <v>1634</v>
       </c>
       <c r="E42" t="n">
-        <v>27157</v>
+        <v>16174</v>
       </c>
       <c r="F42" t="n">
-        <v>2012</v>
+        <v>517</v>
       </c>
       <c r="G42" t="n">
-        <v>16.81</v>
+        <v>23.92</v>
       </c>
       <c r="H42" t="n">
-        <v>27.58</v>
+        <v>32.76</v>
       </c>
       <c r="I42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="b">
-        <v>0</v>
-      </c>
-      <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K42" t="n">
+        <v>67629</v>
+      </c>
+      <c r="L42" t="n">
+        <v>1578</v>
+      </c>
       <c r="M42" t="n">
-        <v>1824125</v>
+        <v>2179622</v>
       </c>
       <c r="N42" t="n">
-        <v>14.23</v>
+        <v>21.46</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -2496,43 +2532,43 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Idaho</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>44030</v>
+        <v>44031</v>
       </c>
       <c r="C43" t="n">
-        <v>14302</v>
+        <v>161575</v>
       </c>
       <c r="D43" t="n">
-        <v>114</v>
+        <v>7295</v>
       </c>
       <c r="E43" t="n">
-        <v>177</v>
+        <v>27157</v>
       </c>
       <c r="F43" t="n">
-        <v>1</v>
+        <v>2012</v>
       </c>
       <c r="G43" t="n">
-        <v>1.24</v>
+        <v>16.81</v>
       </c>
       <c r="H43" t="n">
-        <v>0.88</v>
+        <v>27.58</v>
       </c>
       <c r="I43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="n">
-        <v>11536</v>
+        <v>1824125</v>
       </c>
       <c r="N43" t="n">
-        <v>0.68</v>
+        <v>14.23</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -2543,32 +2579,32 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Idaho</t>
         </is>
       </c>
       <c r="B44" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C44" t="n">
-        <v>46204</v>
+        <v>14873</v>
       </c>
       <c r="D44" t="n">
-        <v>1541</v>
+        <v>114</v>
       </c>
       <c r="E44" t="n">
-        <v>9345</v>
+        <v>191</v>
       </c>
       <c r="F44" t="n">
-        <v>151</v>
+        <v>1</v>
       </c>
       <c r="G44" t="n">
-        <v>20.23</v>
+        <v>1.28</v>
       </c>
       <c r="H44" t="n">
-        <v>9.800000000000001</v>
+        <v>0.88</v>
       </c>
       <c r="I44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" t="b">
         <v>1</v>
@@ -2576,10 +2612,10 @@
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="n">
-        <v>342186</v>
+        <v>11536</v>
       </c>
       <c r="N44" t="n">
-        <v>6.19</v>
+        <v>0.68</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -2590,43 +2626,43 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="B45" s="2" t="n">
         <v>44031</v>
       </c>
       <c r="C45" t="n">
-        <v>113534</v>
+        <v>46204</v>
       </c>
       <c r="D45" t="n">
-        <v>8431</v>
+        <v>1541</v>
       </c>
       <c r="E45" t="n">
-        <v>10663</v>
+        <v>9345</v>
       </c>
       <c r="F45" t="n">
-        <v>691</v>
+        <v>151</v>
       </c>
       <c r="G45" t="n">
-        <v>9.390000000000001</v>
+        <v>20.23</v>
       </c>
       <c r="H45" t="n">
-        <v>8.199999999999999</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="I45" t="b">
         <v>1</v>
       </c>
       <c r="J45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="n">
-        <v>510558</v>
+        <v>342186</v>
       </c>
       <c r="N45" t="n">
-        <v>7.48</v>
+        <v>6.19</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -2637,47 +2673,43 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Wisconsin -- Milwaukee</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="B46" s="2" t="n">
-        <v>44029</v>
+        <v>44031</v>
       </c>
       <c r="C46" t="n">
-        <v>15426</v>
+        <v>113534</v>
       </c>
       <c r="D46" t="n">
-        <v>365</v>
+        <v>8431</v>
       </c>
       <c r="E46" t="n">
-        <v>4438</v>
+        <v>10663</v>
       </c>
       <c r="F46" t="n">
-        <v>146</v>
+        <v>691</v>
       </c>
       <c r="G46" t="n">
-        <v>30.97</v>
+        <v>9.390000000000001</v>
       </c>
       <c r="H46" t="n">
-        <v>40</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="I46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" t="b">
         <v>0</v>
       </c>
-      <c r="K46" t="n">
-        <v>14328</v>
-      </c>
-      <c r="L46" t="n">
-        <v>365</v>
-      </c>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
       <c r="M46" t="n">
-        <v>252321</v>
+        <v>510558</v>
       </c>
       <c r="N46" t="n">
-        <v>26.44</v>
+        <v>7.48</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -2688,49 +2720,100 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>Wisconsin -- Milwaukee</t>
+        </is>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>44029</v>
+      </c>
+      <c r="C47" t="n">
+        <v>15426</v>
+      </c>
+      <c r="D47" t="n">
+        <v>365</v>
+      </c>
+      <c r="E47" t="n">
+        <v>4438</v>
+      </c>
+      <c r="F47" t="n">
+        <v>146</v>
+      </c>
+      <c r="G47" t="n">
+        <v>30.97</v>
+      </c>
+      <c r="H47" t="n">
+        <v>40</v>
+      </c>
+      <c r="I47" t="b">
+        <v>0</v>
+      </c>
+      <c r="J47" t="b">
+        <v>0</v>
+      </c>
+      <c r="K47" t="n">
+        <v>14328</v>
+      </c>
+      <c r="L47" t="n">
+        <v>365</v>
+      </c>
+      <c r="M47" t="n">
+        <v>252321</v>
+      </c>
+      <c r="N47" t="n">
+        <v>26.44</v>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
           <t>Missouri</t>
         </is>
       </c>
-      <c r="B47" s="2" t="n">
-        <v>44031</v>
-      </c>
-      <c r="C47" t="n">
+      <c r="B48" s="2" t="n">
+        <v>44031</v>
+      </c>
+      <c r="C48" t="n">
         <v>33093</v>
       </c>
-      <c r="D47" t="n">
+      <c r="D48" t="n">
         <v>1129</v>
       </c>
-      <c r="E47" t="n">
+      <c r="E48" t="n">
         <v>7705</v>
       </c>
-      <c r="F47" t="n">
+      <c r="F48" t="n">
         <v>380</v>
       </c>
-      <c r="G47" t="n">
+      <c r="G48" t="n">
         <v>30.09</v>
       </c>
-      <c r="H47" t="n">
+      <c r="H48" t="n">
         <v>35.06</v>
       </c>
-      <c r="I47" t="b">
-        <v>0</v>
-      </c>
-      <c r="J47" t="b">
-        <v>1</v>
-      </c>
-      <c r="K47" t="n">
+      <c r="I48" t="b">
+        <v>0</v>
+      </c>
+      <c r="J48" t="b">
+        <v>1</v>
+      </c>
+      <c r="K48" t="n">
         <v>25607</v>
       </c>
-      <c r="L47" t="n">
+      <c r="L48" t="n">
         <v>1084</v>
       </c>
-      <c r="M47" t="n">
+      <c r="M48" t="n">
         <v>704896</v>
       </c>
-      <c r="N47" t="n">
+      <c r="N48" t="n">
         <v>11.57</v>
       </c>
-      <c r="O47" t="inlineStr">
+      <c r="O48" t="inlineStr">
         <is>
           <t>Success!</t>
         </is>

</xml_diff>